<commit_message>
Rename Requirements.txt to requirements.txt
</commit_message>
<xml_diff>
--- a/Schedule/Sample Data/schedule.xlsx
+++ b/Schedule/Sample Data/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dell-my.sharepoint.com/personal/jaga_karunanithi_dellteam_com1/Documents/Solvedesktop/solvedesktop/Schedule/Sample Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="11_F25DC773A252ABDACC104882691943CC5ADE58FF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{115504F2-C822-4C2F-826F-9C5BFB8A8129}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="11_F25DC773A252ABDACC104882691943CC5ADE58FF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0E2CA23-4EA0-4F78-ACFD-74F152C0250F}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="7230" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,25 +33,25 @@
     <t>name</t>
   </si>
   <si>
-    <t>nickname</t>
-  </si>
-  <si>
     <t>918870092425</t>
   </si>
   <si>
     <t>Jagasabarivel</t>
   </si>
   <si>
-    <t>Jaga</t>
-  </si>
-  <si>
     <t>919865975793</t>
   </si>
   <si>
     <t>Shwetha</t>
   </si>
   <si>
-    <t>Shwe</t>
+    <t>charge</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>40</t>
   </si>
 </sst>
 </file>
@@ -403,26 +403,26 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Add template support on whatsapp
</commit_message>
<xml_diff>
--- a/Schedule/Sample Data/schedule.xlsx
+++ b/Schedule/Sample Data/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dell-my.sharepoint.com/personal/jaga_karunanithi_dellteam_com1/Documents/Solvedesktop/solvedesktop/Schedule/Sample Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="11_F25DC773A252ABDACC104882691943CC5ADE58FF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0E2CA23-4EA0-4F78-ACFD-74F152C0250F}"/>
+  <xr:revisionPtr revIDLastSave="38" documentId="11_F25DC773A252ABDACC104882691943CC5ADE58FF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{943D35C9-1353-4816-92AC-A5043C82502D}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="7230" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,33 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>Phone</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>918870092425</t>
   </si>
   <si>
-    <t>Jagasabarivel</t>
-  </si>
-  <si>
     <t>919865975793</t>
   </si>
   <si>
-    <t>Shwetha</t>
-  </si>
-  <si>
-    <t>charge</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>40</t>
+    <t>financial_year</t>
+  </si>
+  <si>
+    <t>final_date</t>
+  </si>
+  <si>
+    <t>2025-26</t>
+  </si>
+  <si>
+    <t>31.03.2025</t>
   </si>
 </sst>
 </file>
@@ -390,7 +384,7 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="12.734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.62890625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.41796875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.734375" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.83984375" style="2"/>
   </cols>
@@ -400,32 +394,32 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>